<commit_message>
feat: add industry into import graduation students
</commit_message>
<xml_diff>
--- a/public/templates/graduation_students_template.xlsx
+++ b/public/templates/graduation_students_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hueph\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Mã sinh viên</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>lehongquang99@gmail.com</t>
+  </si>
+  <si>
+    <t>Mã ngành</t>
+  </si>
+  <si>
+    <t>Tên ngành</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
   </si>
 </sst>
 </file>
@@ -378,19 +387,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +419,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>633773</v>
       </c>
@@ -419,6 +438,12 @@
       </c>
       <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="F2">
+        <v>7480201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add citizen_identification to import graduation excel
</commit_message>
<xml_diff>
--- a/public/templates/graduation_students_template.xlsx
+++ b/public/templates/graduation_students_template.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hueph\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29525"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{259EEE23-FBF4-4110-ABBC-0546B8B901EE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Mã sinh viên</t>
   </si>
@@ -32,7 +39,7 @@
     <t>Họ và tên</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email</t>
+    <t> Email</t>
   </si>
   <si>
     <t>Điểm trung bình</t>
@@ -41,7 +48,13 @@
     <t>Xếp Loại</t>
   </si>
   <si>
-    <t>3.6</t>
+    <t>Mã ngành</t>
+  </si>
+  <si>
+    <t>Tên ngành</t>
+  </si>
+  <si>
+    <t>Căn cước công dân</t>
   </si>
   <si>
     <t>Lê Hồng Quang</t>
@@ -50,36 +63,41 @@
     <t>lehongquang99@gmail.com</t>
   </si>
   <si>
-    <t>Mã ngành</t>
-  </si>
-  <si>
-    <t>Tên ngành</t>
+    <t xml:space="preserve">
+</t>
   </si>
   <si>
     <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>0123456789</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="163"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,21 +116,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -135,39 +175,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -200,9 +240,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -235,6 +292,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -296,13 +370,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -311,6 +378,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -375,7 +449,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -386,69 +480,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="23.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="23.25">
+      <c r="A2" s="1">
+        <v>622222</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>633773</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
         <v>7480201</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{03F7F1E5-541A-4723-BA42-9C2247939D88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add phone_number to import graduations
</commit_message>
<xml_diff>
--- a/public/templates/graduation_students_template.xlsx
+++ b/public/templates/graduation_students_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29525"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{259EEE23-FBF4-4110-ABBC-0546B8B901EE}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE07CDD-88BB-440A-8280-0532B1DE19AE}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mã sinh viên</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Căn cước công dân</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
   </si>
   <si>
     <t>Lê Hồng Quang</t>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t>0123456789</t>
+  </si>
+  <si>
+    <t>0987654321</t>
   </si>
 </sst>
 </file>
@@ -481,20 +487,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25">
+    <row r="1" spans="1:9" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,31 +528,37 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="23.25">
+    <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="1">
         <v>622222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>3.6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1">
         <v>7480201</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>